<commit_message>
Bug fixes in certificate
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/UI_CERTIFICATE_REGISTRATION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/UI_CERTIFICATE_REGISTRATION_HISTORY_DATA.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
@@ -1289,30 +1289,84 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="5" t="inlineStr">
         <is>
           <t>2021-10-20</t>
         </is>
       </c>
       <c r="B30" s="10" t="n">
-        <v>44489.73675903975</v>
-      </c>
-      <c r="C30" t="inlineStr">
+        <v>44489.73675903936</v>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
         <is>
           <t>1511</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>50</v>
-      </c>
-      <c r="E30" t="n">
+      <c r="D30" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" s="5" t="n">
         <v>3.01</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
+          <t>2021-10-21</t>
+        </is>
+      </c>
+      <c r="B31" s="10" t="n">
+        <v>44490.45557141204</v>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2021-10-21</t>
+        </is>
+      </c>
+      <c r="B32" s="10" t="n">
+        <v>44490.46612804689</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>11511</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>50</v>
+      </c>
+      <c r="E32" t="n">
+        <v>51</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="1048559" ht="12.8" customHeight="1" s="6"/>

</xml_diff>

<commit_message>
Certificate Script Support to Prod
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/UI_CERTIFICATE_REGISTRATION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/UI_CERTIFICATE_REGISTRATION_HISTORY_DATA.xlsx
@@ -1397,29 +1397,29 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>2021-10-28</t>
         </is>
       </c>
       <c r="B34" s="10" t="n">
-        <v>44497.41234502867</v>
-      </c>
-      <c r="C34" t="inlineStr">
+        <v>44497.41234502315</v>
+      </c>
+      <c r="C34" s="5" t="inlineStr">
         <is>
           <t>152fnl</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D34" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F34" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" s="5" t="n">
         <v>2.87</v>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
@@ -2113,6 +2113,60 @@
       </c>
       <c r="G11" s="5" t="n">
         <v>8.390000000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>2021-11-03</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>44503.48433738426</v>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>152ccan</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-11-03</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>44503.48806614619</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>152ccaan</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>51</v>
+      </c>
+      <c r="E13" t="n">
+        <v>51</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2.26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registartion Scripts supports in live
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/UI_CERTIFICATE_REGISTRATION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/UI_CERTIFICATE_REGISTRATION_HISTORY_DATA.xlsx
@@ -19,9 +19,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -88,7 +89,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -117,6 +118,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2072,29 +2074,29 @@
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1" s="6">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="5" t="inlineStr">
         <is>
           <t>2022-09-06</t>
         </is>
       </c>
       <c r="B59" s="9" t="n">
-        <v>44810.9392168561</v>
-      </c>
-      <c r="C59" t="inlineStr">
+        <v>44810.93921685185</v>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
         <is>
           <t>cert89</t>
         </is>
       </c>
-      <c r="D59" t="n">
-        <v>51</v>
-      </c>
-      <c r="E59" t="n">
-        <v>51</v>
-      </c>
-      <c r="F59" t="n">
+      <c r="D59" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="E59" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="F59" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G59" t="n">
+      <c r="G59" s="5" t="n">
         <v>1.15</v>
       </c>
     </row>
@@ -2466,7 +2468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
@@ -2896,6 +2898,60 @@
       </c>
       <c r="G15" s="5" t="n">
         <v>5.75</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>2022-09-08</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>44812.4908575463</v>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>cert166</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>51</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2022-09-08</t>
+        </is>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>44812.5083360391</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>certi166</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>51</v>
+      </c>
+      <c r="E17" t="n">
+        <v>51</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>